<commit_message>
The testing excel document updated
</commit_message>
<xml_diff>
--- a/TestingExcel.xlsx
+++ b/TestingExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roqit-my.sharepoint.com/personal/matt_livesey_roq_co_uk/Documents/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roqit-my.sharepoint.com/personal/matt_livesey_roq_co_uk/Documents/Microsoft Teams Chat Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="8_{2947EA06-2B61-4A1C-95B8-CD70305FBCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53C6882A-5254-4FB1-BFE5-5E42722C0263}"/>
+  <xr:revisionPtr revIDLastSave="467" documentId="8_{2947EA06-2B61-4A1C-95B8-CD70305FBCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4DA939F-9CC1-4318-9978-9D459CE3AAE4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{61EC60B6-8976-457E-B6F5-186501E00140}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{61EC60B6-8976-457E-B6F5-186501E00140}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontend" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="150">
   <si>
     <t>User Story</t>
   </si>
@@ -49,6 +49,9 @@
     <t>Test</t>
   </si>
   <si>
+    <t>Steps</t>
+  </si>
+  <si>
     <t>Test ID</t>
   </si>
   <si>
@@ -67,24 +70,6 @@
     <t>Urgency</t>
   </si>
   <si>
-    <t>As a user I would like to be able to add multiple customers.</t>
-  </si>
-  <si>
-    <t>c792302c</t>
-  </si>
-  <si>
-    <t>Select the button for create new customer on the credersi-vend home page</t>
-  </si>
-  <si>
-    <t>A window should open allowing for the user to input a name.</t>
-  </si>
-  <si>
-    <t>When creating a customer it won't allow for multiple customers with the same name.</t>
-  </si>
-  <si>
-    <t>An error should occur informing a user that a customer already has that name</t>
-  </si>
-  <si>
     <t>As a user i would like to be able to log in  given the correct inputs for username and password used.</t>
   </si>
   <si>
@@ -94,28 +79,415 @@
     <t>Password field is empty when the login page has loaded.</t>
   </si>
   <si>
+    <t>Start up web app, check fields have nothing in the password field</t>
+  </si>
+  <si>
     <t>This should display the passworld field as empty, this would force the user to input the appropriate password.</t>
   </si>
   <si>
+    <t xml:space="preserve">The password field is empty when web app loaded </t>
+  </si>
+  <si>
     <t>Username field is empty when the login page has loaded.</t>
   </si>
   <si>
+    <t>Start up web app, check fields have nothing in the username field</t>
+  </si>
+  <si>
     <t>This should display the username field as empty, this would force the user to input an appropriate username.</t>
   </si>
   <si>
+    <t xml:space="preserve">The username field is empty when the web app is loaded </t>
+  </si>
+  <si>
     <t>User should only be able input appropriate characters within the username field.</t>
   </si>
   <si>
+    <t>Start up web app, select username field, input special characters</t>
+  </si>
+  <si>
     <t xml:space="preserve">A popup message should occur informing the user what characters are allowed to be inputted </t>
   </si>
   <si>
+    <t xml:space="preserve">The special characters are allowed into the field as there is only one current login account it only counts the inputs as incorrect credentials </t>
+  </si>
+  <si>
     <t>leaving the passworld field empty and inputting a user within the user field.</t>
   </si>
   <si>
+    <t>Start up web app, select username field, input an actual user's username login credential, leave password field blank</t>
+  </si>
+  <si>
     <t>A popup message should occur informing the user that the entered combination didn't match</t>
   </si>
   <si>
+    <t xml:space="preserve">The Login failed </t>
+  </si>
+  <si>
     <t>try to log in with empty fields</t>
+  </si>
+  <si>
+    <t>Start up web app, click login button</t>
+  </si>
+  <si>
+    <t>As a user I would like to be able create a machine</t>
+  </si>
+  <si>
+    <t>51817c33</t>
+  </si>
+  <si>
+    <t>When on a customers page click the create machine button</t>
+  </si>
+  <si>
+    <t>Get to the create machine page, click the create machine button</t>
+  </si>
+  <si>
+    <t>The page should change and a new page to enter the information should appear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The test passed and a new input screen appeared when clicked </t>
+  </si>
+  <si>
+    <t>Enter the machine information correctly and create a new machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get to the create machine page, click the create machine button, click ok, see new machine </t>
+  </si>
+  <si>
+    <t>The machine should be created and be visible on the list of machines place</t>
+  </si>
+  <si>
+    <t>The machine was created  and is visible on the list of machine in the selected location</t>
+  </si>
+  <si>
+    <t>Try to create a machine with empty fields</t>
+  </si>
+  <si>
+    <t>A popup error message should be produced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The machine was created with name of undifined </t>
+  </si>
+  <si>
+    <t>Try to create a machine with names that are &gt;100 characters</t>
+  </si>
+  <si>
+    <t>Should stop the input of new characters at the limit</t>
+  </si>
+  <si>
+    <t>The machine was created witht the inputted name just not formatted for the size of the machine name box</t>
+  </si>
+  <si>
+    <t>As a user I would like to be able to create a new location</t>
+  </si>
+  <si>
+    <t>52f500a0</t>
+  </si>
+  <si>
+    <t>From the Customer screen select a customer and click on the create location button.</t>
+  </si>
+  <si>
+    <t>Login, Click  a customer, select create site, fill in fields with desired data, click ok, see new site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should come up with the oppourtunity to input location name and details and then add location </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The location was created with normal data </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user i would like to create a new customer </t>
+  </si>
+  <si>
+    <t>77ea23b0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a customer via the website </t>
+  </si>
+  <si>
+    <t>From the login screen, Log in, click new customer button, fill in desired credentials, click ok button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Once ok button is clicked after data input there should new be an interactable customer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A customer is created </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a customer with only special characters </t>
+  </si>
+  <si>
+    <t>From the login screen, Log in, click new customer button, fill in credentials made up of only special characters, click ok button</t>
+  </si>
+  <si>
+    <t>The special characters are rejected due to their safety risks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A customer is created with the name just including special characters </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a customer with same as a current customer </t>
+  </si>
+  <si>
+    <t>From the login screen, Log in, click new customer button, fill in credentials made up of data the same as an already existing customer, click ok button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The customer is rejected because it has the same details as one that already exists </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A customer was created with a unique UUID and the same exact name </t>
+  </si>
+  <si>
+    <t>Create customer with name of just ""</t>
+  </si>
+  <si>
+    <t>From the login screen, Log in, click new customer button, fill in credentials made up of only (""), click ok button</t>
+  </si>
+  <si>
+    <t>The name of the user will just be ""</t>
+  </si>
+  <si>
+    <t>The website breaks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a customer with an extremely long name </t>
+  </si>
+  <si>
+    <t>From the login screen, Log in, click new customer button fill in credentials made up of a value more than 50 characters long, click ok button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name is rejected as the text will be too long </t>
+  </si>
+  <si>
+    <t>The customer was created witht the inputted name just not formatted for the size of the customer name box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create a customer with the name of just a single space </t>
+  </si>
+  <si>
+    <t>From the login screen, Log in, click new customer button fill in credentials made up of a value of only one press of a space bar, click ok button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name of the user will just be a single space </t>
+  </si>
+  <si>
+    <t>The customer was made with the name only being a singular space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user I would like elements to be interactable and do as intended </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click an existing customer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">From login screen, Login, click an existing customer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The customer will be interactable and lead to the sites under that customer </t>
+  </si>
+  <si>
+    <t>The user is able to click a user and see sites belonging to them</t>
+  </si>
+  <si>
+    <t>Click an existing site</t>
+  </si>
+  <si>
+    <t>From login, Login, click an existing customer, click an existing site</t>
+  </si>
+  <si>
+    <t>The site will be selected and show the location on the site</t>
+  </si>
+  <si>
+    <t>The user is able to click the site and see all the locations on the site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click an existing machine </t>
+  </si>
+  <si>
+    <t>From login, Login, click an existing customer, click an existing site, click a location on the site, click a machine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The machine will be selected and will only give the button to add new machine </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user is able to click a machine </t>
+  </si>
+  <si>
+    <t>Click all the way to the end of the breadcrumb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From login screen, Login, click all existing entities on any given breadcrumb until there are no more entities able to be selected </t>
+  </si>
+  <si>
+    <t>The user will reach the end of the breadcrumb with no issue and be left on an open machine tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user is able to follow </t>
+  </si>
+  <si>
+    <t>Click a previous breadcrumb tab to move to previous node in breadcrumb</t>
+  </si>
+  <si>
+    <t>From login screen, Login, click customer, click site, click customer in the breadcrumb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user will be taken back to the page of the customer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user is able to go back to a previous site page from this </t>
+  </si>
+  <si>
+    <t>Click the back button</t>
+  </si>
+  <si>
+    <t>From the login screen, Login, Click customer, click back button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user will be taken to the previous page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user can return to the immediate previous page </t>
+  </si>
+  <si>
+    <t>Postman</t>
+  </si>
+  <si>
+    <t>As a user I should be able to send a simple request to the database to receive all the customers currently stored in the database and then other requests to either delete, create or find single customers that all have a unique UUID</t>
+  </si>
+  <si>
+    <t>8e1b4122</t>
+  </si>
+  <si>
+    <t>Send a request to the database to obtain the current customers that are stored.</t>
+  </si>
+  <si>
+    <t>Postman should be setup using a bearer token, this can be done by copying from the session cookie which can be found in the browser.</t>
+  </si>
+  <si>
+    <t>Expected to recieve JSON data which displays all the current customers within the database</t>
+  </si>
+  <si>
+    <t>Could obtain the customers within the database.</t>
+  </si>
+  <si>
+    <t>Send a request to the database to find a customer based on the customers UUID</t>
+  </si>
+  <si>
+    <t>setup postman to GET request, then input the database uuid and the customer uuid that the user wants to find</t>
+  </si>
+  <si>
+    <t>Expected to recieve JSON data displaying the customer that has been requested</t>
+  </si>
+  <si>
+    <t>The request located the customer based off their UUID</t>
+  </si>
+  <si>
+    <t>Send a request to the database to delete a customer based on the customers UUID</t>
+  </si>
+  <si>
+    <t>Setup postman with a DELETE request and then input the database UUID and the customers UUID</t>
+  </si>
+  <si>
+    <t>Its expected that the customer will be deleted</t>
+  </si>
+  <si>
+    <t>The customer was deleted from the neo4j database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Send a request to the database to create a new customer </t>
+  </si>
+  <si>
+    <t>Setup postman with a POST request and then setup the appropriate file format and create a new user</t>
+  </si>
+  <si>
+    <t>Expected that the customer is created and is assigned a unique UUID</t>
+  </si>
+  <si>
+    <t>A customer was created with a unique UUID</t>
+  </si>
+  <si>
+    <t>Create multiple customers with the same UUID</t>
+  </si>
+  <si>
+    <t>Setup postman with a POST request to attempt to create multiple users with the same UUID</t>
+  </si>
+  <si>
+    <t>Expected to fail due to the customer having the same UUID as another already on the database</t>
+  </si>
+  <si>
+    <t>The database has allowed for customers to be created with the same UUID</t>
+  </si>
+  <si>
+    <t>As a user I should be able to send a simple request to the database to receive all possible sites which belong to a customer and then other requests to either create, delete or find a single route based on UUID.</t>
+  </si>
+  <si>
+    <t>e816f221</t>
+  </si>
+  <si>
+    <t>A request that will locate all sites for a specific customer.</t>
+  </si>
+  <si>
+    <t>Setup postman with a GET request to attempt to pull all sites that are accociated with a specific customer UUID</t>
+  </si>
+  <si>
+    <t>Expected to show all sites that are accociated with that specific customer UUID</t>
+  </si>
+  <si>
+    <t>All sites were displayed that was accociated with the inputted customer UUID</t>
+  </si>
+  <si>
+    <t>A request to locate a single site for a specific customer UUID</t>
+  </si>
+  <si>
+    <t>setup postman with a GET request to pull a specific site based of the sites UUID</t>
+  </si>
+  <si>
+    <t>Expected to show a specific site relating to the sites UUID</t>
+  </si>
+  <si>
+    <t>An individual site was obtained</t>
+  </si>
+  <si>
+    <t>A test to see if it is possible to create a site with nothing in the address field and name field</t>
+  </si>
+  <si>
+    <t>Setup postman with a POST request to attempt to create a site with blank fields</t>
+  </si>
+  <si>
+    <t>An error message will appear identifying that there is an invalid format for the post request</t>
+  </si>
+  <si>
+    <t>A site was created with invalid address and name field. The UUID was automatically generated</t>
+  </si>
+  <si>
+    <t>A test to see if you can create multiple sites with the same UUID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setup postman with a post request to create a site with the same UUID </t>
+  </si>
+  <si>
+    <t>An error should appear with a 400 "bad request"</t>
+  </si>
+  <si>
+    <t>A site was created with the same UUID as another site</t>
+  </si>
+  <si>
+    <t>Performance Testing - the developer has said that the response time of the site should be at 500ms. However, due to the machines worked on by the tester isn't fast, it's decided to add 50% onto the time so the response time should be below 750ms</t>
+  </si>
+  <si>
+    <t>3610a482</t>
+  </si>
+  <si>
+    <t>A test to make sure that the response time is below 750ms</t>
+  </si>
+  <si>
+    <t>Setup a test in postman to say that you expect the response time to be below 750ms</t>
+  </si>
+  <si>
+    <t>The response time should be below 750ms and the test should pass</t>
+  </si>
+  <si>
+    <t>The response time was below the 750ms that had been set. Which in result meant that it had passed</t>
   </si>
 </sst>
 </file>
@@ -125,7 +497,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,8 +505,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,8 +558,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE699"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -185,6 +602,67 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
@@ -199,19 +677,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -220,7 +685,22 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -228,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -252,35 +732,95 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,177 +1136,772 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21673FC-5CA0-49CA-818E-38D08C29D95C}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="42" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" style="4"/>
-    <col min="5" max="6" width="21.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15" style="3" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="22.7109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="42" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="4"/>
+    <col min="6" max="7" width="21.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="15" style="3" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.15" customHeight="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:10" ht="40.15" customHeight="1">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="55.5" customHeight="1">
-      <c r="A2" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="13" t="s">
+    </row>
+    <row r="2" spans="1:10" ht="76.5">
+      <c r="A2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4">
+      <c r="C2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="15">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:9" ht="60.75">
-      <c r="A3" s="9"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="F2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:10" ht="76.5">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="15">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="9"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" ht="76.5">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="F3" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" ht="106.5">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="15">
+        <v>3</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="76.5">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="15">
+        <v>4</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="76.5">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="15">
+        <v>5</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="60.75">
+      <c r="A7" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="15">
         <v>1</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" ht="76.5">
-      <c r="A6" s="9"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="F7" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="60.75">
+      <c r="C8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="4">
         <v>2</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" ht="76.5">
-      <c r="A7" s="9"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="F8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="45.75">
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="4">
         <v>3</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="76.5">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="4">
+      <c r="F9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="91.5">
+      <c r="C10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="4">
         <v>4</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="76.5">
-      <c r="A9" s="9"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="F10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="76.5">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="60.75">
+      <c r="A12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="60.75">
+      <c r="C13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="60.75">
+      <c r="C14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="45.75">
+      <c r="C15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="4">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="123.75" customHeight="1">
+      <c r="C16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="4">
         <v>5</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="9"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
+      <c r="F16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="123.75" customHeight="1">
+      <c r="C17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="4">
+        <v>6</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="60.75">
+      <c r="A18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="45.75">
+      <c r="C19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="4">
+        <v>2</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="60.75">
+      <c r="C20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="4">
+        <v>3</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="76.5">
+      <c r="C21" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="4">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="45.75">
+      <c r="C22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="4">
+        <v>5</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="45.75">
+      <c r="C23" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="4">
+        <v>6</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="20" customFormat="1">
+      <c r="A24" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+    </row>
+    <row r="25" spans="1:10" ht="32.25" customHeight="1">
+      <c r="A25" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="121.5">
+      <c r="A26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="4">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H26" s="3">
+        <v>44813</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="60.75">
+      <c r="A27" s="33"/>
+      <c r="B27" s="34"/>
+      <c r="C27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="4">
+        <v>2</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H27" s="3">
+        <v>44813</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45.75">
+      <c r="A28" s="33"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" s="4">
+        <v>3</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H28" s="3">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="60.75">
+      <c r="A29" s="33"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E29" s="4">
+        <v>4</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="H29" s="3">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="76.5">
+      <c r="A30" s="33"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E30" s="4">
+        <v>5</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H30" s="3">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="37" customFormat="1">
+      <c r="A31" s="33"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+    </row>
+    <row r="32" spans="1:10" ht="121.5">
+      <c r="A32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="4">
+        <v>1</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H32" s="3">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="45.75">
+      <c r="A33" s="36"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E33" s="4">
+        <v>2</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H33" s="3">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="76.5">
+      <c r="A34" s="36"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="4">
+        <v>3</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H34" s="3">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="45.75">
+      <c r="A35" s="36"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E35" s="4">
+        <v>4</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H35" s="3">
+        <v>44816</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="37" customFormat="1">
+      <c r="A36" s="36"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+    </row>
+    <row r="37" spans="1:10" ht="137.25">
+      <c r="A37" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E37" s="4">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H37" s="3">
+        <v>44816</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -780,7 +1915,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -794,7 +1929,7 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>